<commit_message>
Signed-off-by: Rakesh B 08-02-24
</commit_message>
<xml_diff>
--- a/JDBC_FrameWork/src/test/resources/TestData/DBWorkBook.xlsx
+++ b/JDBC_FrameWork/src/test/resources/TestData/DBWorkBook.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Selenium_Training\JDBC_FrameWork\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\git\JDBC_FrameWork\JDBC_FrameWork\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4605" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="5025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginEmail" sheetId="1" r:id="rId1"/>
     <sheet name="SQLQuery" sheetId="2" r:id="rId2"/>
+    <sheet name="TestSQLQuery" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Engg123@gmail.com</t>
   </si>
@@ -40,6 +41,69 @@
   </si>
   <si>
     <t>select * from logindata where Email=</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>select category_id from category where name='Action';</t>
+  </si>
+  <si>
+    <t>select country_id from city where city='Abha';</t>
+  </si>
+  <si>
+    <t>select payment_id from payment where rental_id='573';</t>
+  </si>
+  <si>
+    <t>select payment_id from payment where rental_id='9100';</t>
+  </si>
+  <si>
+    <t>select first_name from actor where actor_id=82;</t>
+  </si>
+  <si>
+    <t>WOODY</t>
+  </si>
+  <si>
+    <t>select last_update from actor where actor_id=85;</t>
+  </si>
+  <si>
+    <t>15-02-2006  04:34:33</t>
+  </si>
+  <si>
+    <t>select last_update from actor where first_name='BETTE';</t>
+  </si>
+  <si>
+    <t>Select release_year from film group by release_year;</t>
+  </si>
+  <si>
+    <t>Select name from category where category_id=16;</t>
+  </si>
+  <si>
+    <t>Select postal_code from address where postal_code=35200;</t>
+  </si>
+  <si>
+    <t>35200</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>95</t>
   </si>
 </sst>
 </file>
@@ -55,12 +119,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,8 +145,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -410,4 +499,111 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>